<commit_message>
Add xls file downloading, loading and showing
</commit_message>
<xml_diff>
--- a/functions/test.xlsx
+++ b/functions/test.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Cell A1</t>
+    <t xml:space="preserve">Cell A1 mit wichtigen Informationen</t>
   </si>
   <si>
     <t xml:space="preserve">Zelle B1</t>
@@ -40,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,8 +100,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -127,13 +132,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>